<commit_message>
Updated the machine_spec file
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/machine_spec.xlsx
+++ b/mosip_master/xlsx/machine_spec.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh.Binayak\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C32D9E-E4A3-4778-BEBB-461C12B4F221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7CA3B9-EC35-44FF-BF1A-590DAC962822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>lang_code</t>
   </si>
@@ -67,9 +68,6 @@
   </si>
   <si>
     <t>RESIDENT-REG</t>
-  </si>
-  <si>
-    <t>RESIDENT-1</t>
   </si>
 </sst>
 </file>
@@ -455,23 +453,23 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1"/>
+    <col min="8" max="8" width="24.81640625" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,12 +498,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="B2">
+        <v>1001</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated the machine_spec file with id data type to 0 decimal
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/machine_spec.xlsx
+++ b/mosip_master/xlsx/machine_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7CA3B9-EC35-44FF-BF1A-590DAC962822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E96BFCD-7DC0-460B-ABFC-1AAF0E5F5384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -127,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -136,6 +135,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +455,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,7 +475,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -529,6 +531,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added updated machine_spec.xlsx and machine_master.xlsx and machine_master_h.xlsx
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/machine_spec.xlsx
+++ b/mosip_master/xlsx/machine_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B079B67B-6CCF-483C-9AD6-FAB7D8846613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A26D8A9-0DCB-4122-9507-178D5B2F4D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +85,7 @@
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,15 +123,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -456,27 +446,28 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="30.81640625" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.26953125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="24.81640625" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="11.54296875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -497,36 +488,36 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="2">
         <v>1001</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="b">
+      <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>